<commit_message>
update timeline for 26th of october
</commit_message>
<xml_diff>
--- a/Project Timeline.xlsx
+++ b/Project Timeline.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidde\Dropbox\Kieran Third year\BCIT254 Interactive Media Application Development\InteractiveMediaProject\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37725982-33EC-40BE-AABF-8D8A64AEC645}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -27,7 +21,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -195,7 +189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -884,14 +878,26 @@
     <xf numFmtId="2" fontId="22" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -902,6 +908,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -917,72 +956,27 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="20">
-    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="% complete" xfId="16"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
+    <cellStyle name="Activity" xfId="2"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
+    <cellStyle name="Actual legend" xfId="15"/>
     <cellStyle name="Bad" xfId="19" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Percent Complete" xfId="6"/>
+    <cellStyle name="Period Headers" xfId="3"/>
+    <cellStyle name="Period Highlight Control" xfId="7"/>
+    <cellStyle name="Period Value" xfId="13"/>
+    <cellStyle name="Plan legend" xfId="14"/>
+    <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="7">
@@ -1309,15 +1303,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:U35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1338,10 +1332,10 @@
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="48"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="8" t="s">
@@ -1365,54 +1359,54 @@
       <c r="K2" s="12"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="39" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="50"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="39"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="40"/>
     </row>
     <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="22" t="s">
@@ -1440,8 +1434,8 @@
       <c r="K5" s="21"/>
     </row>
     <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="22" t="s">
         <v>17</v>
       </c>
@@ -1467,8 +1461,8 @@
       <c r="K6" s="21"/>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="22" t="s">
         <v>13</v>
       </c>
@@ -1494,8 +1488,8 @@
       <c r="K7" s="21"/>
     </row>
     <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="22" t="s">
         <v>16</v>
       </c>
@@ -1521,8 +1515,8 @@
       <c r="K8" s="21"/>
     </row>
     <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="22" t="s">
         <v>19</v>
       </c>
@@ -1548,7 +1542,7 @@
       <c r="K9" s="21"/>
     </row>
     <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="22" t="s">
         <v>20</v>
       </c>
@@ -1577,8 +1571,8 @@
       <c r="K10" s="21"/>
     </row>
     <row r="11" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="22" t="s">
@@ -1606,8 +1600,8 @@
       <c r="K11" s="21"/>
     </row>
     <row r="12" spans="2:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="22" t="s">
         <v>17</v>
       </c>
@@ -1633,8 +1627,8 @@
       <c r="K12" s="21"/>
     </row>
     <row r="13" spans="2:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="22" t="s">
         <v>16</v>
       </c>
@@ -1660,8 +1654,8 @@
       <c r="K13" s="21"/>
     </row>
     <row r="14" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="22" t="s">
         <v>19</v>
       </c>
@@ -1687,8 +1681,8 @@
       <c r="K14" s="21"/>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="22" t="s">
         <v>18</v>
       </c>
@@ -1714,10 +1708,10 @@
       <c r="K15" s="21"/>
     </row>
     <row r="16" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="34" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="22" t="s">
@@ -1726,126 +1720,162 @@
       <c r="E16" s="14">
         <v>1</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
+      <c r="F16" s="25">
+        <v>43748</v>
+      </c>
+      <c r="G16" s="14">
+        <v>3</v>
+      </c>
+      <c r="H16" s="25">
+        <v>43763</v>
+      </c>
       <c r="I16" s="20">
         <v>43770</v>
       </c>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="21"/>
     </row>
     <row r="17" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="14">
         <v>2</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="13"/>
+      <c r="F17" s="25">
+        <v>43763</v>
+      </c>
+      <c r="G17" s="14">
+        <v>7</v>
+      </c>
+      <c r="H17" s="25">
+        <v>43763</v>
+      </c>
       <c r="I17" s="20">
         <v>43770</v>
       </c>
       <c r="J17" s="14">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="K17" s="21"/>
     </row>
     <row r="18" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="22" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="14">
         <v>3</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
+      <c r="F18" s="25">
+        <v>43764</v>
+      </c>
+      <c r="G18" s="14">
+        <v>2</v>
+      </c>
+      <c r="H18" s="25">
+        <v>43764</v>
+      </c>
       <c r="I18" s="20">
         <v>43770</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="K18" s="21"/>
     </row>
     <row r="19" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="22" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="14">
         <v>4</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="13"/>
+      <c r="F19" s="25">
+        <v>43764</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19" s="25">
+        <v>43764</v>
+      </c>
       <c r="I19" s="20">
         <v>43770</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="K19" s="21"/>
     </row>
     <row r="20" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="22" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="14">
         <v>5</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="13"/>
+      <c r="F20" s="25">
+        <v>43764</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1</v>
+      </c>
+      <c r="H20" s="25">
+        <v>43764</v>
+      </c>
       <c r="I20" s="20">
         <v>43770</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="K20" s="21"/>
     </row>
     <row r="21" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="22" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="14">
         <v>9</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="13"/>
+      <c r="F21" s="25">
+        <v>43764</v>
+      </c>
+      <c r="G21" s="14">
+        <v>1</v>
+      </c>
+      <c r="H21" s="25">
+        <v>43764</v>
+      </c>
       <c r="I21" s="20">
         <v>43770</v>
       </c>
       <c r="J21" s="14">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="K21" s="21"/>
     </row>
     <row r="22" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="22" t="s">
         <v>29</v>
       </c>
@@ -1865,8 +1895,8 @@
       <c r="K22" s="21"/>
     </row>
     <row r="23" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="35"/>
+      <c r="C23" s="34" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="22" t="s">
@@ -1888,8 +1918,8 @@
       <c r="K23" s="21"/>
     </row>
     <row r="24" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="22" t="s">
         <v>40</v>
       </c>
@@ -1909,8 +1939,8 @@
       <c r="K24" s="21"/>
     </row>
     <row r="25" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="22" t="s">
         <v>41</v>
       </c>
@@ -1930,8 +1960,8 @@
       <c r="K25" s="21"/>
     </row>
     <row r="26" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="22" t="s">
         <v>42</v>
       </c>
@@ -1952,8 +1982,8 @@
       <c r="U26" s="13"/>
     </row>
     <row r="27" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="22" t="s">
         <v>35</v>
       </c>
@@ -1973,11 +2003,11 @@
       <c r="K27" s="21"/>
     </row>
     <row r="28" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
-      <c r="C28" s="33" t="s">
+      <c r="B28" s="36"/>
+      <c r="C28" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="34"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="14">
         <v>1</v>
       </c>
@@ -1994,10 +2024,10 @@
       <c r="K28" s="21"/>
     </row>
     <row r="29" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="50" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="22" t="s">
@@ -2014,8 +2044,8 @@
       <c r="K29" s="21"/>
     </row>
     <row r="30" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="31"/>
-      <c r="C30" s="36"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="22" t="s">
         <v>44</v>
       </c>
@@ -2035,8 +2065,8 @@
       <c r="K30" s="21"/>
     </row>
     <row r="31" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="31"/>
-      <c r="C31" s="36"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="51"/>
       <c r="D31" s="22" t="s">
         <v>39</v>
       </c>
@@ -2056,8 +2086,8 @@
       <c r="K31" s="21"/>
     </row>
     <row r="32" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="31"/>
-      <c r="C32" s="36"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="51"/>
       <c r="D32" s="22" t="s">
         <v>43</v>
       </c>
@@ -2077,8 +2107,8 @@
       <c r="K32" s="21"/>
     </row>
     <row r="33" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="31"/>
-      <c r="C33" s="37"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="22" t="s">
         <v>39</v>
       </c>
@@ -2098,7 +2128,7 @@
       <c r="K33" s="21"/>
     </row>
     <row r="34" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="32"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="23" t="s">
         <v>45</v>
       </c>
@@ -2128,20 +2158,33 @@
         <f>SUM(E5:E34)</f>
         <v>90</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="29"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="47"/>
       <c r="I35" s="18"/>
       <c r="J35" s="19">
         <f>SUM(J5:J34)</f>
-        <v>-75.5</v>
+        <v>-60.5</v>
       </c>
       <c r="K35" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="B16:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="E3:E4"/>
@@ -2150,19 +2193,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="C11:C15"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C16:C22"/>
-    <mergeCell ref="B16:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C33"/>
   </mergeCells>
   <conditionalFormatting sqref="K35 B35:F35">
     <cfRule type="expression" dxfId="6" priority="17">
@@ -2248,13 +2278,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A2" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="C3:D3 B3:B4" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="G3:G4 H3:J3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="K3:K4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B2:D2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="C3:D3 B3:B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="E3:E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="F3:F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="G3:G4 H3:J3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="K3:K4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B2:D2"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>